<commit_message>
updated to 30 day
</commit_message>
<xml_diff>
--- a/App/assets/csv/vari.xlsx
+++ b/App/assets/csv/vari.xlsx
@@ -147,43 +147,43 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2.6635396058275347e-06</v>
+        <v>2.66077495065119e-06</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1.8196363647243167e-05</v>
+        <v>1.8270840137369382e-05</v>
       </c>
       <c r="E2">
-        <v>5.5242520691164011e-05</v>
+        <v>5.5661580657220136e-05</v>
       </c>
       <c r="F2">
-        <v>3.9271409536702657e-05</v>
+        <v>3.9382838159013105e-05</v>
       </c>
       <c r="G2">
-        <v>9.5869189526071784e-05</v>
+        <v>9.5358201627691923e-05</v>
       </c>
       <c r="H2">
-        <v>3.4572622561825619e-05</v>
+        <v>3.4292045866939637e-05</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>2.7967942771070912e-06</v>
+        <v>3.0767179580759817e-06</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>2.6959030395541082e-06</v>
+        <v>2.4282307200008546e-06</v>
       </c>
       <c r="M2">
-        <v>1.2339684855488621e-05</v>
+        <v>1.2434706797846496e-05</v>
       </c>
       <c r="N2">
-        <v>8.1606014265919102e-06</v>
+        <v>8.7719837069164931e-06</v>
       </c>
     </row>
     <row r="3">
@@ -235,43 +235,43 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1.8196363647243167e-05</v>
+        <v>1.8270840137369382e-05</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.013901375829840346</v>
+        <v>0.013901285286847613</v>
       </c>
       <c r="E4">
-        <v>0.0033533961757202979</v>
+        <v>0.0033357821563100121</v>
       </c>
       <c r="F4">
-        <v>0.0030316304209954468</v>
+        <v>0.0030481107468282426</v>
       </c>
       <c r="G4">
-        <v>0.0024104068369515891</v>
+        <v>0.0024215041316008358</v>
       </c>
       <c r="H4">
-        <v>0.0026803231094741456</v>
+        <v>0.0026872637217823193</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0.00014377823873820385</v>
+        <v>0.00014122209205041583</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0.0027551407618145616</v>
+        <v>0.0027476351096986933</v>
       </c>
       <c r="M4">
-        <v>0.00294328987545865</v>
+        <v>0.0029408724756072708</v>
       </c>
       <c r="N4">
-        <v>0.0031328874715461485</v>
+        <v>0.0031141388852496095</v>
       </c>
     </row>
     <row r="5">
@@ -279,43 +279,43 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5.5242520691164011e-05</v>
+        <v>5.5661580657220136e-05</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.0033533961757202979</v>
+        <v>0.0033357821563100121</v>
       </c>
       <c r="E5">
-        <v>0.015759486364052503</v>
+        <v>0.015760719856752457</v>
       </c>
       <c r="F5">
-        <v>0.0035928973303157156</v>
+        <v>0.0036862847448876743</v>
       </c>
       <c r="G5">
-        <v>0.0040202819391199109</v>
+        <v>0.0040633307155682214</v>
       </c>
       <c r="H5">
-        <v>0.0030450196601260063</v>
+        <v>0.0030513419363144005</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0.00070185717939901752</v>
+        <v>0.00071269536380637994</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0.001767598791190185</v>
+        <v>0.0017486337614127199</v>
       </c>
       <c r="M5">
-        <v>0.0012530218302137389</v>
+        <v>0.0012564027847564295</v>
       </c>
       <c r="N5">
-        <v>0.0017122565244603863</v>
+        <v>0.001650942170062722</v>
       </c>
     </row>
     <row r="6">
@@ -323,43 +323,43 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.9271409536702657e-05</v>
+        <v>3.9382838159013105e-05</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.0030316304209954468</v>
+        <v>0.0030481107468282426</v>
       </c>
       <c r="E6">
-        <v>0.0035928973303157156</v>
+        <v>0.0036862847448876743</v>
       </c>
       <c r="F6">
-        <v>0.060471308705733362</v>
+        <v>0.056893024387214837</v>
       </c>
       <c r="G6">
-        <v>0.0039237853975239156</v>
+        <v>0.0040375259219165268</v>
       </c>
       <c r="H6">
-        <v>0.0031717739757387764</v>
+        <v>0.0032329808639281017</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.0017856722863370926</v>
+        <v>0.0018482774601927604</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0.0016755747435897625</v>
+        <v>0.0016467974788365422</v>
       </c>
       <c r="M6">
-        <v>0.0016800996097713291</v>
+        <v>0.00160547644205672</v>
       </c>
       <c r="N6">
-        <v>0.00030000997985215927</v>
+        <v>0.00014721508230219812</v>
       </c>
     </row>
     <row r="7">
@@ -367,43 +367,43 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>9.5869189526071784e-05</v>
+        <v>9.5358201627691923e-05</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0.0024104068369515891</v>
+        <v>0.0024215041316008358</v>
       </c>
       <c r="E7">
-        <v>0.0040202819391199109</v>
+        <v>0.0040633307155682214</v>
       </c>
       <c r="F7">
-        <v>0.0039237853975239156</v>
+        <v>0.0040375259219165268</v>
       </c>
       <c r="G7">
-        <v>1.0163381283350366</v>
+        <v>1.0163260748983445</v>
       </c>
       <c r="H7">
-        <v>0.0063806929718852644</v>
+        <v>0.0063673897205753305</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>-0.0021158866291835767</v>
+        <v>-0.0020682260958636441</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0.00045182689790279786</v>
+        <v>0.00042771780957028926</v>
       </c>
       <c r="M7">
-        <v>0.0013287350845307461</v>
+        <v>0.001321315562316739</v>
       </c>
       <c r="N7">
-        <v>-0.0079178558171809702</v>
+        <v>-0.0079254329278459282</v>
       </c>
     </row>
     <row r="8">
@@ -411,43 +411,43 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>3.4572622561825619e-05</v>
+        <v>3.4292045866939637e-05</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0.0026803231094741456</v>
+        <v>0.0026872637217823193</v>
       </c>
       <c r="E8">
-        <v>0.0030450196601260063</v>
+        <v>0.0030513419363144005</v>
       </c>
       <c r="F8">
-        <v>0.0031717739757387764</v>
+        <v>0.0032329808639281017</v>
       </c>
       <c r="G8">
-        <v>0.0063806929718852644</v>
+        <v>0.0063673897205753305</v>
       </c>
       <c r="H8">
-        <v>0.042732116149947222</v>
+        <v>0.042719684018940295</v>
       </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>-0.00090454208493381827</v>
+        <v>-0.00087908490247774068</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.00088791825450977927</v>
+        <v>0.00087701947842297478</v>
       </c>
       <c r="M8">
-        <v>0.0015954048675131279</v>
+        <v>0.001593242931765482</v>
       </c>
       <c r="N8">
-        <v>-0.0020839833524427605</v>
+        <v>-0.0020810214270282684</v>
       </c>
     </row>
     <row r="9">
@@ -499,43 +499,43 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2.7967942771070912e-06</v>
+        <v>3.0767179580759817e-06</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.00014377823873820385</v>
+        <v>0.00014122209205041583</v>
       </c>
       <c r="E10">
-        <v>0.00070185717939901752</v>
+        <v>0.00071269536380637994</v>
       </c>
       <c r="F10">
-        <v>0.0017856722863370926</v>
+        <v>0.0018482774601927604</v>
       </c>
       <c r="G10">
-        <v>-0.0021158866291835767</v>
+        <v>-0.0020682260958636441</v>
       </c>
       <c r="H10">
-        <v>-0.00090454208493381827</v>
+        <v>-0.00087908490247774068</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0.0067029160260348329</v>
+        <v>0.0066910429376094496</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>-6.7305242700204057e-05</v>
+        <v>-6.8560370320828521e-05</v>
       </c>
       <c r="M10">
-        <v>-0.00052788481041198855</v>
+        <v>-0.00052846027743836451</v>
       </c>
       <c r="N10">
-        <v>-0.00057303225889487788</v>
+        <v>-0.00061094219507482907</v>
       </c>
     </row>
     <row r="11">
@@ -587,43 +587,43 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>2.6959030395541082e-06</v>
+        <v>2.4282307200008546e-06</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.0027551407618145616</v>
+        <v>0.0027476351096986933</v>
       </c>
       <c r="E12">
-        <v>0.001767598791190185</v>
+        <v>0.0017486337614127199</v>
       </c>
       <c r="F12">
-        <v>0.0016755747435897625</v>
+        <v>0.0016467974788365422</v>
       </c>
       <c r="G12">
-        <v>0.00045182689790279786</v>
+        <v>0.00042771780957028926</v>
       </c>
       <c r="H12">
-        <v>0.00088791825450977927</v>
+        <v>0.00087701947842297478</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
-        <v>-6.7305242700204057e-05</v>
+        <v>-6.8560370320828521e-05</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0.011719825652425311</v>
+        <v>0.011671356801518673</v>
       </c>
       <c r="M12">
-        <v>0.0064310913817721485</v>
+        <v>0.0063898907082341611</v>
       </c>
       <c r="N12">
-        <v>0.0066219667001040016</v>
+        <v>0.0065834648456979924</v>
       </c>
     </row>
     <row r="13">
@@ -631,43 +631,43 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>1.2339684855488621e-05</v>
+        <v>1.2434706797846496e-05</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>0.00294328987545865</v>
+        <v>0.0029408724756072708</v>
       </c>
       <c r="E13">
-        <v>0.0012530218302137389</v>
+        <v>0.0012564027847564295</v>
       </c>
       <c r="F13">
-        <v>0.0016800996097713291</v>
+        <v>0.00160547644205672</v>
       </c>
       <c r="G13">
-        <v>0.0013287350845307461</v>
+        <v>0.001321315562316739</v>
       </c>
       <c r="H13">
-        <v>0.0015954048675131279</v>
+        <v>0.001593242931765482</v>
       </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
-        <v>-0.00052788481041198855</v>
+        <v>-0.00052846027743836451</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
       <c r="L13">
-        <v>0.0064310913817721485</v>
+        <v>0.0063898907082341611</v>
       </c>
       <c r="M13">
-        <v>0.013600288999331812</v>
+        <v>0.013556369739288629</v>
       </c>
       <c r="N13">
-        <v>0.0065104860561749798</v>
+        <v>0.0064810362319701774</v>
       </c>
     </row>
     <row r="14">
@@ -675,43 +675,43 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>8.1606014265919102e-06</v>
+        <v>8.7719837069164931e-06</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0.0031328874715461485</v>
+        <v>0.0031141388852496095</v>
       </c>
       <c r="E14">
-        <v>0.0017122565244603863</v>
+        <v>0.001650942170062722</v>
       </c>
       <c r="F14">
-        <v>0.00030000997985215927</v>
+        <v>0.00014721508230219812</v>
       </c>
       <c r="G14">
-        <v>-0.0079178558171809702</v>
+        <v>-0.0079254329278459282</v>
       </c>
       <c r="H14">
-        <v>-0.0020839833524427605</v>
+        <v>-0.0020810214270282684</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
-        <v>-0.00057303225889487788</v>
+        <v>-0.00061094219507482907</v>
       </c>
       <c r="K14">
         <v>0</v>
       </c>
       <c r="L14">
-        <v>0.0066219667001040016</v>
+        <v>0.0065834648456979924</v>
       </c>
       <c r="M14">
-        <v>0.0065104860561749798</v>
+        <v>0.0064810362319701774</v>
       </c>
       <c r="N14">
-        <v>0.015363960827907345</v>
+        <v>0.015350002739102564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>